<commit_message>
updates number_type for several numeric attributes
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_carcass_metadata.xlsx
+++ b/data-raw/metadata/yuba_carcass_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B95DAB9-FE09-6942-91B5-293DA19BF026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7B7F4A-97E4-054F-BEF5-F74511072FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68640" yWindow="-9480" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -156,13 +156,16 @@
   <si>
     <t>Whether or not the fish had spawned. Levels = c("spawned", "unspawned", NA)</t>
   </si>
+  <si>
+    <t>integer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -223,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -249,14 +252,13 @@
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +478,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -654,7 +656,9 @@
       <c r="G4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="5"/>
       <c r="K4" s="11"/>
@@ -814,14 +818,16 @@
       <c r="G8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="18">
+      <c r="L8" s="5">
         <v>1</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="5">
         <v>35</v>
       </c>
       <c r="N8" s="1"/>

</xml_diff>

<commit_message>
updates metadata files to reflect new data files - new standard format
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_carcass_metadata.xlsx
+++ b/data-raw/metadata/yuba_carcass_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7B7F4A-97E4-054F-BEF5-F74511072FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31898A12-7B89-5C41-86F8-E7CB530EDDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="-9480" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>Run of carcass observed.</t>
   </si>
 </sst>
 </file>
@@ -474,11 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -798,38 +804,28 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>34</v>
+      <c r="B8" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
-        <v>35</v>
-      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -845,19 +841,39 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <v>35</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -884,8 +900,8 @@
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -912,8 +928,8 @@
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -996,8 +1012,8 @@
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1025,7 +1041,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="12"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1080,7 +1096,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="10"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="5"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1098,18 +1114,18 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1208,8 +1224,9 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -1235,9 +1252,8 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
@@ -1405,34 +1421,34 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1464,29 +1480,39 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1505,16 +1531,6 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1645,6 +1661,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1672,7 +1689,6 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1700,6 +1716,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1727,7 +1744,6 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2679,7 +2695,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
@@ -28606,18 +28622,46 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
+    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="3"/>
+      <c r="G1001" s="3"/>
+      <c r="H1001" s="3"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="3"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="3"/>
+      <c r="M1001" s="3"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C57:C1000 C33:C45 C1:C31" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C1:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E33:E1000 E1:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E1:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F33:F1000 F1:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F1:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33:H1000 H1:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H1:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>